<commit_message>
Update cac tinh nang va sua loi
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
+++ b/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
@@ -41,7 +41,7 @@
     <t>2. Vị trí, đơn vị công tác: Văn phòng - Hải quan cửa khẩu quốc tế Cầu Treo</t>
   </si>
   <si>
-    <t>3. Số ngày làm việc theo quy định của pháp luật lao động trong tháng: 23</t>
+    <t>3. Số ngày làm việc theo quy định của pháp luật lao động trong tháng: 0</t>
   </si>
   <si>
     <t>4. Số ngày nghỉ trong tháng (có phép): 0</t>
@@ -53,10 +53,10 @@
     <t>6. Số lần vi phạm quy chế, quy định: 0</t>
   </si>
   <si>
-    <t>7. Hành vi vi phạm: 0</t>
-  </si>
-  <si>
-    <t>8. Hình thức kỷ luật: 0</t>
+    <t xml:space="preserve">7. Hành vi vi phạm: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Hình thức kỷ luật: </t>
   </si>
   <si>
     <t>9. Bảng kê chi tiết công việc:</t>

</xml_diff>

<commit_message>
Update Chức năng nhiều đội phó quản lý 1 cán bộ
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
+++ b/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>CỤC HẢI QUAN TỈNH HÀ TĨNH</t>
   </si>
@@ -41,7 +41,7 @@
     <t>2. Vị trí, đơn vị công tác: Văn phòng - Hải quan cửa khẩu quốc tế Cầu Treo</t>
   </si>
   <si>
-    <t>3. Số ngày làm việc theo quy định của pháp luật lao động trong tháng: 0</t>
+    <t>3. Số ngày làm việc theo quy định của pháp luật lao động trong tháng: 23</t>
   </si>
   <si>
     <t>4. Số ngày nghỉ trong tháng (có phép): 0</t>
@@ -53,10 +53,10 @@
     <t>6. Số lần vi phạm quy chế, quy định: 0</t>
   </si>
   <si>
-    <t xml:space="preserve">7. Hành vi vi phạm: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Hình thức kỷ luật: </t>
+    <t>7. Hành vi vi phạm: 0</t>
+  </si>
+  <si>
+    <t>8. Hình thức kỷ luật: 0</t>
   </si>
   <si>
     <t>9. Bảng kê chi tiết công việc:</t>
@@ -104,40 +104,25 @@
     <t>Đánh máy</t>
   </si>
   <si>
-    <t>16/03/2025</t>
-  </si>
-  <si>
-    <t>18/03/2025</t>
-  </si>
-  <si>
-    <t>update...</t>
+    <t>26/03/2025</t>
+  </si>
+  <si>
+    <t>updating...</t>
   </si>
   <si>
     <t>Vượt tiến độ hoặc có chất lượng hoặc hiệu quả cao</t>
   </si>
   <si>
+    <t>Đúng tiến độ, đảm bảo chất lượng và hiệu quả</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Hải</t>
+  </si>
+  <si>
     <t>Chưa đảm bảo về yêu cầu và chất lượng</t>
   </si>
   <si>
-    <t>Nguyễn Văn Hải</t>
-  </si>
-  <si>
-    <t>Họp chi bộ</t>
-  </si>
-  <si>
-    <t>17/03/2025</t>
-  </si>
-  <si>
-    <t>Công văn 322</t>
-  </si>
-  <si>
-    <t>Chan Dan</t>
-  </si>
-  <si>
-    <t>19/03/2025</t>
-  </si>
-  <si>
-    <t>Nguyễn Hiếu</t>
+    <t>Nguyễn Duy Cường</t>
   </si>
   <si>
     <t>10. Kết quả xếp loại chất lượng tháng:</t>
@@ -529,10 +514,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A15" sqref="A15:M18"/>
+      <selection activeCell="A15" sqref="A15:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -678,113 +663,39 @@
         <v>29</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="G17" s="5" t="s">
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
         <v>37</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>1</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cập nhật và sửa lỗi cac chuc nang moi nhat
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
+++ b/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>CỤC HẢI QUAN TỈNH HÀ TĨNH</t>
   </si>
@@ -146,13 +146,16 @@
     <t>Chưa đánh giá</t>
   </si>
   <si>
+    <t>Không đảm bảo chất lượng</t>
+  </si>
+  <si>
+    <t>22/03/2025</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
     <t>Nguyễn Duy Cường</t>
-  </si>
-  <si>
-    <t>22/03/2025</t>
-  </si>
-  <si>
-    <t>abcd</t>
   </si>
   <si>
     <t>10. Kết quả xếp loại chất lượng tháng:</t>
@@ -723,7 +726,7 @@
         <v>33</v>
       </c>
       <c r="M16" s="5">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>36</v>
@@ -804,13 +807,13 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="M18" s="5">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="O18" s="5"/>
     </row>
@@ -848,21 +851,21 @@
         <v>33</v>
       </c>
       <c r="M19" s="5">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="O19" s="5"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4.Fix load thông tin mục xuất lịch sử theo tháng
</commit_message>
<xml_diff>
--- a/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
+++ b/public/temp/evaluation_report_03_2025_hieunguyen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>CỤC HẢI QUAN TỈNH HÀ TĨNH</t>
   </si>
@@ -41,22 +41,22 @@
     <t>2. Vị trí, đơn vị công tác: Văn phòng - Chi cục Hải quan khu vực IX</t>
   </si>
   <si>
-    <t>3. Số ngày làm việc theo quy định của pháp luật lao động trong tháng: 0</t>
-  </si>
-  <si>
-    <t>4. Số ngày nghỉ trong tháng (có phép): 0</t>
-  </si>
-  <si>
-    <t>5. Số ngày nghỉ trong tháng (không phép): 0</t>
-  </si>
-  <si>
-    <t>6. Số lần vi phạm quy chế, quy định: 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. Hành vi vi phạm: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Hình thức kỷ luật: </t>
+    <t>3. Số ngày làm việc theo quy định của pháp luật lao động trong tháng: 28</t>
+  </si>
+  <si>
+    <t>4. Số ngày nghỉ trong tháng (có phép): 2</t>
+  </si>
+  <si>
+    <t>5. Số ngày nghỉ trong tháng (không phép): 2</t>
+  </si>
+  <si>
+    <t>6. Số lần vi phạm quy chế, quy định: 1</t>
+  </si>
+  <si>
+    <t>7. Hành vi vi phạm: aaaa</t>
+  </si>
+  <si>
+    <t>8. Hình thức kỷ luật: cccc</t>
   </si>
   <si>
     <t>9. Bảng kê chi tiết công việc:</t>
@@ -125,7 +125,7 @@
     <t>Nguyễn Văn Hải</t>
   </si>
   <si>
-    <t>Chan Dan</t>
+    <t>Bùi Thanh San</t>
   </si>
   <si>
     <t>Họp chi bộ</t>
@@ -155,7 +155,19 @@
     <t>abcd</t>
   </si>
   <si>
-    <t>Nguyễn Duy Cường</t>
+    <t>Nguyễn Đình Long</t>
+  </si>
+  <si>
+    <t>31/03/2025</t>
+  </si>
+  <si>
+    <t>05/04/2025</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>Chưa phê duyệt</t>
   </si>
   <si>
     <t>10. Kết quả xếp loại chất lượng tháng:</t>
@@ -547,10 +559,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A15" sqref="A15:O19"/>
+      <selection activeCell="A15" sqref="A15:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -858,14 +870,53 @@
       </c>
       <c r="O19" s="5"/>
     </row>
-    <row r="21" spans="1:15">
-      <c r="A21" t="s">
+    <row r="20" spans="1:15">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="D20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="5">
+        <v>95</v>
+      </c>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>